<commit_message>
work in progress: ML training class
</commit_message>
<xml_diff>
--- a/diabetes_init_train.xlsx
+++ b/diabetes_init_train.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baltschuler/Desktop/Harvard/Senior Year/CS 262/decentralized_federated_learning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neeraj/repos/decentralized_federated_learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86B46DD-9AA2-C84D-A834-1A818CD38D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83D4346-929A-A24D-8E42-08C4AEECB657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="5180" windowWidth="27240" windowHeight="16440" xr2:uid="{85DC1203-E8A2-934A-96D9-987AA363DDBA}"/>
+    <workbookView xWindow="1560" yWindow="500" windowWidth="27240" windowHeight="16140" xr2:uid="{85DC1203-E8A2-934A-96D9-987AA363DDBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -384,8 +384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58AD745F-0EE2-4F4E-9108-FB3A4B7B5085}">
   <dimension ref="A1:I526"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I526"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>